<commit_message>
adding class 03 and 04
</commit_message>
<xml_diff>
--- a/Class 02/Action Table.xlsx
+++ b/Class 02/Action Table.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\python-immersion\Class 02\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6E3E468-EC53-4A07-8B4B-9A6CAEBAE7CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67EEFE8D-AC9A-486C-A475-AE4110CB4DF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -19,13 +19,7 @@
     <sheet name="Total" sheetId="2" r:id="rId4"/>
     <sheet name="Ticker" sheetId="3" r:id="rId5"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">Analysis!$A$10:$A$62</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">Analysis!$C$10:$C$62</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">Analysis!$C$9</definedName>
-  </definedNames>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -43,7 +37,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -65,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1522" uniqueCount="1082">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1523" uniqueCount="1082">
   <si>
     <t>Var. Sem. (%)</t>
   </si>
@@ -3569,7 +3563,7 @@
     <xf numFmtId="0" fontId="7" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -3735,6 +3729,11 @@
               <a:effectLst/>
               <a:sp3d/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000001-FF49-4491-B83D-7E21E8DCF00D}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="1"/>
@@ -3772,6 +3771,11 @@
               <a:effectLst/>
               <a:sp3d/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000003-FF49-4491-B83D-7E21E8DCF00D}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="2"/>
@@ -3809,6 +3813,11 @@
               <a:effectLst/>
               <a:sp3d/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000005-FF49-4491-B83D-7E21E8DCF00D}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="3"/>
@@ -3846,6 +3855,11 @@
               <a:effectLst/>
               <a:sp3d/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000007-FF49-4491-B83D-7E21E8DCF00D}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="4"/>
@@ -3883,6 +3897,11 @@
               <a:effectLst/>
               <a:sp3d/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000009-FF49-4491-B83D-7E21E8DCF00D}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="5"/>
@@ -3920,6 +3939,11 @@
               <a:effectLst/>
               <a:sp3d/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000B-FF49-4491-B83D-7E21E8DCF00D}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="6"/>
@@ -3960,6 +3984,11 @@
               <a:effectLst/>
               <a:sp3d/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000D-FF49-4491-B83D-7E21E8DCF00D}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="7"/>
@@ -4000,6 +4029,11 @@
               <a:effectLst/>
               <a:sp3d/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000F-FF49-4491-B83D-7E21E8DCF00D}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="8"/>
@@ -4040,6 +4074,11 @@
               <a:effectLst/>
               <a:sp3d/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000011-FF49-4491-B83D-7E21E8DCF00D}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="9"/>
@@ -4080,6 +4119,11 @@
               <a:effectLst/>
               <a:sp3d/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000013-FF49-4491-B83D-7E21E8DCF00D}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="10"/>
@@ -4120,6 +4164,11 @@
               <a:effectLst/>
               <a:sp3d/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000015-FF49-4491-B83D-7E21E8DCF00D}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="11"/>
@@ -4160,6 +4209,11 @@
               <a:effectLst/>
               <a:sp3d/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000017-FF49-4491-B83D-7E21E8DCF00D}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="12"/>
@@ -4203,6 +4257,11 @@
               <a:effectLst/>
               <a:sp3d/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000019-FF49-4491-B83D-7E21E8DCF00D}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="13"/>
@@ -4246,6 +4305,11 @@
               <a:effectLst/>
               <a:sp3d/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000001B-FF49-4491-B83D-7E21E8DCF00D}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="14"/>
@@ -4289,6 +4353,11 @@
               <a:effectLst/>
               <a:sp3d/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000001D-FF49-4491-B83D-7E21E8DCF00D}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="15"/>
@@ -4332,6 +4401,11 @@
               <a:effectLst/>
               <a:sp3d/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000001F-FF49-4491-B83D-7E21E8DCF00D}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="16"/>
@@ -4375,6 +4449,11 @@
               <a:effectLst/>
               <a:sp3d/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000021-FF49-4491-B83D-7E21E8DCF00D}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="17"/>
@@ -4418,6 +4497,11 @@
               <a:effectLst/>
               <a:sp3d/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000023-FF49-4491-B83D-7E21E8DCF00D}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="18"/>
@@ -4458,6 +4542,11 @@
               <a:effectLst/>
               <a:sp3d/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000025-FF49-4491-B83D-7E21E8DCF00D}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="19"/>
@@ -4498,6 +4587,11 @@
               <a:effectLst/>
               <a:sp3d/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000027-FF49-4491-B83D-7E21E8DCF00D}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="20"/>
@@ -4538,6 +4632,11 @@
               <a:effectLst/>
               <a:sp3d/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000029-FF49-4491-B83D-7E21E8DCF00D}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="21"/>
@@ -4578,6 +4677,11 @@
               <a:effectLst/>
               <a:sp3d/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000002B-FF49-4491-B83D-7E21E8DCF00D}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="22"/>
@@ -4618,6 +4722,11 @@
               <a:effectLst/>
               <a:sp3d/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000002D-FF49-4491-B83D-7E21E8DCF00D}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="23"/>
@@ -4658,6 +4767,11 @@
               <a:effectLst/>
               <a:sp3d/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000002F-FF49-4491-B83D-7E21E8DCF00D}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="24"/>
@@ -4701,6 +4815,11 @@
               <a:effectLst/>
               <a:sp3d/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000031-FF49-4491-B83D-7E21E8DCF00D}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="25"/>
@@ -4744,6 +4863,11 @@
               <a:effectLst/>
               <a:sp3d/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000033-FF49-4491-B83D-7E21E8DCF00D}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="26"/>
@@ -4787,6 +4911,11 @@
               <a:effectLst/>
               <a:sp3d/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000035-FF49-4491-B83D-7E21E8DCF00D}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="27"/>
@@ -4830,6 +4959,11 @@
               <a:effectLst/>
               <a:sp3d/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000037-FF49-4491-B83D-7E21E8DCF00D}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="28"/>
@@ -4873,6 +5007,11 @@
               <a:effectLst/>
               <a:sp3d/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000039-FF49-4491-B83D-7E21E8DCF00D}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="29"/>
@@ -4916,6 +5055,11 @@
               <a:effectLst/>
               <a:sp3d/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000003B-FF49-4491-B83D-7E21E8DCF00D}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="30"/>
@@ -4956,6 +5100,11 @@
               <a:effectLst/>
               <a:sp3d/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000003D-FF49-4491-B83D-7E21E8DCF00D}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="31"/>
@@ -4996,6 +5145,11 @@
               <a:effectLst/>
               <a:sp3d/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000003F-FF49-4491-B83D-7E21E8DCF00D}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="32"/>
@@ -5036,6 +5190,11 @@
               <a:effectLst/>
               <a:sp3d/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000041-FF49-4491-B83D-7E21E8DCF00D}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="33"/>
@@ -5076,6 +5235,11 @@
               <a:effectLst/>
               <a:sp3d/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000043-FF49-4491-B83D-7E21E8DCF00D}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="34"/>
@@ -5116,6 +5280,11 @@
               <a:effectLst/>
               <a:sp3d/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000045-FF49-4491-B83D-7E21E8DCF00D}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="35"/>
@@ -5156,6 +5325,11 @@
               <a:effectLst/>
               <a:sp3d/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000047-FF49-4491-B83D-7E21E8DCF00D}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="36"/>
@@ -5199,6 +5373,11 @@
               <a:effectLst/>
               <a:sp3d/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000049-FF49-4491-B83D-7E21E8DCF00D}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="37"/>
@@ -5242,6 +5421,11 @@
               <a:effectLst/>
               <a:sp3d/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000004B-FF49-4491-B83D-7E21E8DCF00D}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="38"/>
@@ -5285,6 +5469,11 @@
               <a:effectLst/>
               <a:sp3d/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000004D-FF49-4491-B83D-7E21E8DCF00D}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="39"/>
@@ -5328,6 +5517,11 @@
               <a:effectLst/>
               <a:sp3d/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000004F-FF49-4491-B83D-7E21E8DCF00D}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="40"/>
@@ -5371,6 +5565,11 @@
               <a:effectLst/>
               <a:sp3d/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000051-FF49-4491-B83D-7E21E8DCF00D}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="41"/>
@@ -5414,6 +5613,11 @@
               <a:effectLst/>
               <a:sp3d/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000053-FF49-4491-B83D-7E21E8DCF00D}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="42"/>
@@ -5454,6 +5658,11 @@
               <a:effectLst/>
               <a:sp3d/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000055-FF49-4491-B83D-7E21E8DCF00D}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="43"/>
@@ -5494,6 +5703,11 @@
               <a:effectLst/>
               <a:sp3d/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000057-FF49-4491-B83D-7E21E8DCF00D}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="44"/>
@@ -5534,6 +5748,11 @@
               <a:effectLst/>
               <a:sp3d/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000059-FF49-4491-B83D-7E21E8DCF00D}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="45"/>
@@ -5574,6 +5793,11 @@
               <a:effectLst/>
               <a:sp3d/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000005B-FF49-4491-B83D-7E21E8DCF00D}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="46"/>
@@ -5614,6 +5838,11 @@
               <a:effectLst/>
               <a:sp3d/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000005D-FF49-4491-B83D-7E21E8DCF00D}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="47"/>
@@ -5654,6 +5883,11 @@
               <a:effectLst/>
               <a:sp3d/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000005F-FF49-4491-B83D-7E21E8DCF00D}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="48"/>
@@ -5697,6 +5931,11 @@
               <a:effectLst/>
               <a:sp3d/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000061-FF49-4491-B83D-7E21E8DCF00D}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="49"/>
@@ -5740,6 +5979,11 @@
               <a:effectLst/>
               <a:sp3d/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000063-FF49-4491-B83D-7E21E8DCF00D}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="50"/>
@@ -5783,6 +6027,11 @@
               <a:effectLst/>
               <a:sp3d/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000065-FF49-4491-B83D-7E21E8DCF00D}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="51"/>
@@ -5826,6 +6075,11 @@
               <a:effectLst/>
               <a:sp3d/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000067-FF49-4491-B83D-7E21E8DCF00D}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="52"/>
@@ -5869,6 +6123,11 @@
               <a:effectLst/>
               <a:sp3d/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000069-FF49-4491-B83D-7E21E8DCF00D}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:cat>
             <c:strRef>
@@ -7910,9 +8169,7 @@
   </sheetPr>
   <dimension ref="A1:T1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="O8" sqref="O8"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
@@ -25611,8 +25868,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE9D32CA-5E2D-40A2-B2A2-36E8BB183494}">
   <dimension ref="A1:C86"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C80" sqref="C80"/>
+    <sheetView topLeftCell="A61" workbookViewId="0">
+      <selection activeCell="C73" sqref="C73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -26535,7 +26792,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20D9FD77-5119-453F-BB01-7F56CA505E69}">
-  <dimension ref="A1:B81"/>
+  <dimension ref="A1:C81"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -26547,652 +26804,895 @@
     <col min="2" max="2" width="38.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15">
+    <row r="1" spans="1:3" ht="15">
       <c r="A1" s="20" t="s">
         <v>1079</v>
       </c>
       <c r="B1" s="20" t="s">
         <v>1058</v>
       </c>
-    </row>
-    <row r="2" spans="1:2">
+      <c r="C1" s="20" t="s">
+        <v>1072</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
       <c r="A2" t="s">
         <v>181</v>
       </c>
       <c r="B2" t="s">
         <v>1004</v>
       </c>
-    </row>
-    <row r="3" spans="1:2">
+      <c r="C2">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
       <c r="A3" t="s">
         <v>232</v>
       </c>
       <c r="B3" t="s">
         <v>1005</v>
       </c>
-    </row>
-    <row r="4" spans="1:2">
+      <c r="C3">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
       <c r="A4" t="s">
         <v>179</v>
       </c>
       <c r="B4" t="s">
         <v>1006</v>
       </c>
-    </row>
-    <row r="5" spans="1:2">
+      <c r="C4">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
       <c r="A5" t="s">
         <v>263</v>
       </c>
       <c r="B5" t="s">
         <v>1007</v>
       </c>
-    </row>
-    <row r="6" spans="1:2">
+      <c r="C5">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
       <c r="A6" t="s">
         <v>305</v>
       </c>
       <c r="B6" t="s">
         <v>1008</v>
       </c>
-    </row>
-    <row r="7" spans="1:2">
+      <c r="C6">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
       <c r="A7" t="s">
         <v>210</v>
       </c>
       <c r="B7" t="s">
         <v>1006</v>
       </c>
-    </row>
-    <row r="8" spans="1:2">
+      <c r="C7">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
       <c r="A8" t="s">
         <v>179</v>
       </c>
       <c r="B8" t="s">
         <v>1006</v>
       </c>
-    </row>
-    <row r="9" spans="1:2">
+      <c r="C8">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
       <c r="A9" t="s">
         <v>184</v>
       </c>
       <c r="B9" t="s">
         <v>1005</v>
       </c>
-    </row>
-    <row r="10" spans="1:2">
+      <c r="C9">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
       <c r="A10" t="s">
         <v>247</v>
       </c>
       <c r="B10" t="s">
         <v>1009</v>
       </c>
-    </row>
-    <row r="11" spans="1:2">
+      <c r="C10">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
       <c r="A11" t="s">
         <v>190</v>
       </c>
       <c r="B11" t="s">
         <v>1010</v>
       </c>
-    </row>
-    <row r="12" spans="1:2">
+      <c r="C11">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
       <c r="A12" t="s">
         <v>282</v>
       </c>
       <c r="B12" t="s">
         <v>1011</v>
       </c>
-    </row>
-    <row r="13" spans="1:2">
+      <c r="C12">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
       <c r="A13" t="s">
         <v>297</v>
       </c>
       <c r="B13" t="s">
         <v>1012</v>
       </c>
-    </row>
-    <row r="14" spans="1:2">
+      <c r="C13">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
       <c r="A14" t="s">
         <v>187</v>
       </c>
       <c r="B14" t="s">
         <v>1013</v>
       </c>
-    </row>
-    <row r="15" spans="1:2">
+      <c r="C14">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
       <c r="A15" t="s">
         <v>279</v>
       </c>
       <c r="B15" t="s">
         <v>1006</v>
       </c>
-    </row>
-    <row r="16" spans="1:2">
+      <c r="C15">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
       <c r="A16" t="s">
         <v>195</v>
       </c>
       <c r="B16" t="s">
         <v>1008</v>
       </c>
-    </row>
-    <row r="17" spans="1:2">
+      <c r="C16">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
       <c r="A17" t="s">
         <v>220</v>
       </c>
       <c r="B17" t="s">
         <v>1004</v>
       </c>
-    </row>
-    <row r="18" spans="1:2">
+      <c r="C17">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
       <c r="A18" t="s">
         <v>259</v>
       </c>
       <c r="B18" t="s">
         <v>1014</v>
       </c>
-    </row>
-    <row r="19" spans="1:2">
+      <c r="C18">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
       <c r="A19" t="s">
         <v>246</v>
       </c>
       <c r="B19" t="s">
         <v>1015</v>
       </c>
-    </row>
-    <row r="20" spans="1:2">
+      <c r="C19">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
       <c r="A20" t="s">
         <v>192</v>
       </c>
       <c r="B20" t="s">
         <v>1016</v>
       </c>
-    </row>
-    <row r="21" spans="1:2">
+      <c r="C20">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
       <c r="A21" t="s">
         <v>253</v>
       </c>
       <c r="B21" t="s">
         <v>1017</v>
       </c>
-    </row>
-    <row r="22" spans="1:2">
+      <c r="C21">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
       <c r="A22" t="s">
         <v>186</v>
       </c>
       <c r="B22" t="s">
         <v>1010</v>
       </c>
-    </row>
-    <row r="23" spans="1:2">
+      <c r="C22">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
       <c r="A23" t="s">
         <v>221</v>
       </c>
       <c r="B23" t="s">
         <v>1018</v>
       </c>
-    </row>
-    <row r="24" spans="1:2">
+      <c r="C23">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
       <c r="A24" t="s">
         <v>227</v>
       </c>
       <c r="B24" t="s">
         <v>1019</v>
       </c>
-    </row>
-    <row r="25" spans="1:2">
+      <c r="C24">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3">
       <c r="A25" t="s">
         <v>212</v>
       </c>
       <c r="B25" t="s">
         <v>1020</v>
       </c>
-    </row>
-    <row r="26" spans="1:2">
+      <c r="C25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3">
       <c r="A26" t="s">
         <v>332</v>
       </c>
       <c r="B26" t="s">
         <v>1021</v>
       </c>
-    </row>
-    <row r="27" spans="1:2">
+      <c r="C26">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3">
       <c r="A27" t="s">
         <v>209</v>
       </c>
       <c r="B27" t="s">
         <v>1022</v>
       </c>
-    </row>
-    <row r="28" spans="1:2">
+      <c r="C27">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3">
       <c r="A28" t="s">
         <v>183</v>
       </c>
       <c r="B28" t="s">
         <v>1023</v>
       </c>
-    </row>
-    <row r="29" spans="1:2">
+      <c r="C28">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3">
       <c r="A29" t="s">
         <v>278</v>
       </c>
       <c r="B29" t="s">
         <v>1024</v>
       </c>
-    </row>
-    <row r="30" spans="1:2">
+      <c r="C29">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3">
       <c r="A30" t="s">
         <v>249</v>
       </c>
       <c r="B30" t="s">
         <v>1021</v>
       </c>
-    </row>
-    <row r="31" spans="1:2">
+      <c r="C30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3">
       <c r="A31" t="s">
         <v>266</v>
       </c>
       <c r="B31" t="s">
         <v>1025</v>
       </c>
-    </row>
-    <row r="32" spans="1:2">
+      <c r="C31">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3">
       <c r="A32" t="s">
         <v>201</v>
       </c>
       <c r="B32" t="s">
         <v>1026</v>
       </c>
-    </row>
-    <row r="33" spans="1:2">
+      <c r="C32">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3">
       <c r="A33" t="s">
         <v>292</v>
       </c>
       <c r="B33" t="s">
         <v>1006</v>
       </c>
-    </row>
-    <row r="34" spans="1:2">
+      <c r="C33">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3">
       <c r="A34" t="s">
         <v>189</v>
       </c>
       <c r="B34" t="s">
         <v>1025</v>
       </c>
-    </row>
-    <row r="35" spans="1:2">
+      <c r="C34">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3">
       <c r="A35" t="s">
         <v>206</v>
       </c>
       <c r="B35" t="s">
         <v>1010</v>
       </c>
-    </row>
-    <row r="36" spans="1:2">
+      <c r="C35">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3">
       <c r="A36" t="s">
         <v>244</v>
       </c>
       <c r="B36" t="s">
         <v>1027</v>
       </c>
-    </row>
-    <row r="37" spans="1:2">
+      <c r="C36">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3">
       <c r="A37" t="s">
         <v>248</v>
       </c>
       <c r="B37" t="s">
         <v>1004</v>
       </c>
-    </row>
-    <row r="38" spans="1:2">
+      <c r="C37">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3">
       <c r="A38" t="s">
         <v>296</v>
       </c>
       <c r="B38" t="s">
         <v>1028</v>
       </c>
-    </row>
-    <row r="39" spans="1:2">
+      <c r="C38">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3">
       <c r="A39" t="s">
         <v>314</v>
       </c>
       <c r="B39" t="s">
         <v>1018</v>
       </c>
-    </row>
-    <row r="40" spans="1:2">
+      <c r="C39">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3">
       <c r="A40" t="s">
         <v>177</v>
       </c>
       <c r="B40" t="s">
         <v>1029</v>
       </c>
-    </row>
-    <row r="41" spans="1:2">
+      <c r="C40">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3">
       <c r="A41" t="s">
         <v>186</v>
       </c>
       <c r="B41" t="s">
         <v>1010</v>
       </c>
-    </row>
-    <row r="42" spans="1:2">
+      <c r="C41">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3">
       <c r="A42" t="s">
         <v>229</v>
       </c>
       <c r="B42" t="s">
         <v>1004</v>
       </c>
-    </row>
-    <row r="43" spans="1:2">
+      <c r="C42">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3">
       <c r="A43" t="s">
         <v>226</v>
       </c>
       <c r="B43" t="s">
         <v>1030</v>
       </c>
-    </row>
-    <row r="44" spans="1:2">
+      <c r="C43">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3">
       <c r="A44" t="s">
         <v>202</v>
       </c>
       <c r="B44" t="s">
         <v>1008</v>
       </c>
-    </row>
-    <row r="45" spans="1:2">
+      <c r="C44">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3">
       <c r="A45" t="s">
         <v>228</v>
       </c>
       <c r="B45" t="s">
         <v>1031</v>
       </c>
-    </row>
-    <row r="46" spans="1:2">
+      <c r="C45">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3">
       <c r="A46" t="s">
         <v>241</v>
       </c>
       <c r="B46" t="s">
         <v>1018</v>
       </c>
-    </row>
-    <row r="47" spans="1:2">
+      <c r="C46">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3">
       <c r="A47" t="s">
         <v>213</v>
       </c>
       <c r="B47" t="s">
         <v>1032</v>
       </c>
-    </row>
-    <row r="48" spans="1:2">
+      <c r="C47">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3">
       <c r="A48" t="s">
         <v>269</v>
       </c>
       <c r="B48" t="s">
         <v>1033</v>
       </c>
-    </row>
-    <row r="49" spans="1:2">
+      <c r="C48">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3">
       <c r="A49" t="s">
         <v>315</v>
       </c>
       <c r="B49" t="s">
         <v>1034</v>
       </c>
-    </row>
-    <row r="50" spans="1:2">
+      <c r="C49">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3">
       <c r="A50" t="s">
         <v>325</v>
       </c>
       <c r="B50" t="s">
         <v>1035</v>
       </c>
-    </row>
-    <row r="51" spans="1:2">
+      <c r="C50">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3">
       <c r="A51" t="s">
         <v>223</v>
       </c>
       <c r="B51" t="s">
         <v>1008</v>
       </c>
-    </row>
-    <row r="52" spans="1:2">
+      <c r="C51">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3">
       <c r="A52" t="s">
         <v>281</v>
       </c>
       <c r="B52" t="s">
         <v>1008</v>
       </c>
-    </row>
-    <row r="53" spans="1:2">
+      <c r="C52">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3">
       <c r="A53" t="s">
         <v>291</v>
       </c>
       <c r="B53" t="s">
         <v>1036</v>
       </c>
-    </row>
-    <row r="54" spans="1:2">
+      <c r="C53">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3">
       <c r="A54" t="s">
         <v>245</v>
       </c>
       <c r="B54" t="s">
         <v>1037</v>
       </c>
-    </row>
-    <row r="55" spans="1:2">
+      <c r="C54">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3">
       <c r="A55" t="s">
         <v>319</v>
       </c>
       <c r="B55" t="s">
         <v>1038</v>
       </c>
-    </row>
-    <row r="56" spans="1:2">
+      <c r="C55">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3">
       <c r="A56" t="s">
         <v>115</v>
       </c>
       <c r="B56" t="s">
         <v>1024</v>
       </c>
-    </row>
-    <row r="57" spans="1:2">
+      <c r="C56">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3">
       <c r="A57" t="s">
         <v>295</v>
       </c>
       <c r="B57" t="s">
         <v>1039</v>
       </c>
-    </row>
-    <row r="58" spans="1:2">
+      <c r="C57">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3">
       <c r="A58" t="s">
         <v>188</v>
       </c>
       <c r="B58" t="s">
         <v>1014</v>
       </c>
-    </row>
-    <row r="59" spans="1:2">
+      <c r="C58">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3">
       <c r="A59" t="s">
         <v>349</v>
       </c>
       <c r="B59" t="s">
         <v>1040</v>
       </c>
-    </row>
-    <row r="60" spans="1:2">
+      <c r="C59">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3">
       <c r="A60" t="s">
         <v>350</v>
       </c>
       <c r="B60" t="s">
         <v>1041</v>
       </c>
-    </row>
-    <row r="61" spans="1:2">
+      <c r="C60">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3">
       <c r="A61" t="s">
         <v>288</v>
       </c>
       <c r="B61" t="s">
         <v>1036</v>
       </c>
-    </row>
-    <row r="62" spans="1:2">
+      <c r="C61">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3">
       <c r="A62" t="s">
         <v>309</v>
       </c>
       <c r="B62" t="s">
         <v>1042</v>
       </c>
-    </row>
-    <row r="63" spans="1:2">
+      <c r="C62">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3">
       <c r="A63" t="s">
         <v>191</v>
       </c>
       <c r="B63" t="s">
         <v>1043</v>
       </c>
-    </row>
-    <row r="64" spans="1:2">
+      <c r="C63">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3">
       <c r="A64" t="s">
         <v>324</v>
       </c>
       <c r="B64" t="s">
         <v>1044</v>
       </c>
-    </row>
-    <row r="65" spans="1:2">
+      <c r="C64">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3">
       <c r="A65" t="s">
         <v>300</v>
       </c>
       <c r="B65" t="s">
         <v>1045</v>
       </c>
-    </row>
-    <row r="66" spans="1:2">
+      <c r="C65">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3">
       <c r="A66" t="s">
         <v>205</v>
       </c>
       <c r="B66" t="s">
         <v>1046</v>
       </c>
-    </row>
-    <row r="67" spans="1:2">
+      <c r="C66">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3">
       <c r="A67" t="s">
         <v>318</v>
       </c>
       <c r="B67" t="s">
         <v>1017</v>
       </c>
-    </row>
-    <row r="68" spans="1:2">
+      <c r="C67">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3">
       <c r="A68" t="s">
         <v>237</v>
       </c>
       <c r="B68" t="s">
         <v>1044</v>
       </c>
-    </row>
-    <row r="69" spans="1:2">
+      <c r="C68">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3">
       <c r="A69" t="s">
         <v>280</v>
       </c>
       <c r="B69" t="s">
         <v>1047</v>
       </c>
-    </row>
-    <row r="70" spans="1:2">
+      <c r="C69">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3">
       <c r="A70" t="s">
         <v>193</v>
       </c>
       <c r="B70" t="s">
         <v>1048</v>
       </c>
-    </row>
-    <row r="71" spans="1:2">
+      <c r="C70">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3">
       <c r="A71" t="s">
         <v>222</v>
       </c>
       <c r="B71" t="s">
         <v>1049</v>
       </c>
-    </row>
-    <row r="72" spans="1:2">
+      <c r="C71">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3">
       <c r="A72" t="s">
         <v>180</v>
       </c>
       <c r="B72" t="s">
         <v>1050</v>
       </c>
-    </row>
-    <row r="73" spans="1:2">
+      <c r="C72">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3">
       <c r="A73" t="s">
         <v>256</v>
       </c>
       <c r="B73" t="s">
         <v>1051</v>
       </c>
-    </row>
-    <row r="74" spans="1:2">
+      <c r="C73">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3">
       <c r="A74" t="s">
         <v>283</v>
       </c>
       <c r="B74" t="s">
         <v>1052</v>
       </c>
-    </row>
-    <row r="75" spans="1:2">
+      <c r="C74">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3">
       <c r="A75" t="s">
         <v>178</v>
       </c>
       <c r="B75" t="s">
         <v>1053</v>
       </c>
-    </row>
-    <row r="76" spans="1:2">
+      <c r="C75">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3">
       <c r="A76" t="s">
         <v>194</v>
       </c>
       <c r="B76" t="s">
         <v>1046</v>
       </c>
-    </row>
-    <row r="77" spans="1:2">
+      <c r="C76">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3">
       <c r="A77" t="s">
         <v>252</v>
       </c>
       <c r="B77" t="s">
         <v>1019</v>
       </c>
-    </row>
-    <row r="78" spans="1:2">
+      <c r="C77">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3">
       <c r="A78" t="s">
         <v>262</v>
       </c>
       <c r="B78" t="s">
         <v>1054</v>
       </c>
-    </row>
-    <row r="79" spans="1:2">
+      <c r="C78">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3">
       <c r="A79" t="s">
         <v>196</v>
       </c>
       <c r="B79" t="s">
         <v>1055</v>
       </c>
-    </row>
-    <row r="80" spans="1:2">
+      <c r="C79">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3">
       <c r="A80" t="s">
         <v>182</v>
       </c>
       <c r="B80" t="s">
         <v>1056</v>
       </c>
-    </row>
-    <row r="81" spans="1:2">
+      <c r="C80">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3">
       <c r="A81" t="s">
         <v>185</v>
       </c>
       <c r="B81" t="s">
         <v>1013</v>
+      </c>
+      <c r="C81">
+        <v>132</v>
       </c>
     </row>
   </sheetData>
@@ -27208,7 +27708,7 @@
   <dimension ref="A1:B1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="12.75"/>

</xml_diff>